<commit_message>
So a little reworking was done here, the biggest thing to note is that I needed to change the map slightly so that the ghosts could move, as their current jail was just a bunch of walls, so i just made them empty tiles as the ghosts break in the top anways when they return home. Fixed the map so I could start my tests, and so far the ones I've made succeed.
</commit_message>
<xml_diff>
--- a/reengineering/src/new/PakuJava/src/asset/map.xlsx
+++ b/reengineering/src/new/PakuJava/src/asset/map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CSSE\se\se3860\firebreathingrubberduckies\reengineering\src\new\PakuJava\src\asset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Videogamer90\Desktop\Reengineering\reengineering\src\new\PakuJava\src\asset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15806948-DF24-4739-BFCD-4A7C9CC494E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC64EABC-EC6E-4A16-B769-C7A6AAAB95A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -880,7 +880,7 @@
   <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,22 +2043,22 @@
         <v>0</v>
       </c>
       <c r="L14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="3">
         <v>0</v>
@@ -2129,22 +2129,22 @@
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R15" s="3">
         <v>0</v>
@@ -2215,22 +2215,22 @@
         <v>0</v>
       </c>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R16" s="3">
         <v>0</v>

</xml_diff>